<commit_message>
Add country code excel
</commit_message>
<xml_diff>
--- a/Country-Code.xlsx
+++ b/Country-Code.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrutimehta/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinge\Desktop\Data Engineer CC4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5E8BA44-4DC3-4FE7-8F1F-665BD731A366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="6260" windowWidth="24440" windowHeight="14500" xr2:uid="{F44E485E-B9EA-7D43-9A7B-5903DA87CF9B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F44E485E-B9EA-7D43-9A7B-5903DA87CF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,9 +131,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -170,7 +171,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -276,7 +277,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,7 +419,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,9 +433,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -442,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -450,7 +455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14</v>
       </c>
@@ -458,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -466,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>37</v>
       </c>
@@ -474,7 +479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>94</v>
       </c>
@@ -482,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>148</v>
       </c>
@@ -490,7 +495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>162</v>
       </c>
@@ -498,7 +503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>166</v>
       </c>
@@ -506,7 +511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>184</v>
       </c>
@@ -514,7 +519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>189</v>
       </c>
@@ -522,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>191</v>
       </c>
@@ -530,7 +535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>208</v>
       </c>
@@ -538,7 +543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>214</v>
       </c>
@@ -546,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>215</v>
       </c>
@@ -554,7 +559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>216</v>
       </c>

</xml_diff>